<commit_message>
Added Test case for Games on sale, modified keyword file "Top Sellers.robot" and added new tab in excel sheet
</commit_message>
<xml_diff>
--- a/GameDetails.xlsx
+++ b/GameDetails.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\PycharmProjects\StoreSteamPowered\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45260788-E134-4A06-BE8D-B0D35ADAE945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBA82D9-72A0-472F-81C2-541A3B26819E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Free to play" sheetId="1" r:id="rId1"/>
+    <sheet name="On Sale" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="125">
   <si>
     <t>Game Names</t>
   </si>
@@ -28,6 +29,9 @@
     <t>Release Date</t>
   </si>
   <si>
+    <t>Game Price</t>
+  </si>
+  <si>
     <t>Game Category</t>
   </si>
   <si>
@@ -43,176 +47,213 @@
     <t>Free to Play</t>
   </si>
   <si>
-    <t>Brawlhalla - All Legends (Current and Future)</t>
-  </si>
-  <si>
-    <t>3 Nov, 2015</t>
+    <t>Brawlhalla - Autumn Championship 2021 Pack</t>
+  </si>
+  <si>
+    <t>30 Sep, 2021</t>
+  </si>
+  <si>
+    <t>CDN$ 49.99</t>
+  </si>
+  <si>
+    <t>Business tour. Great Leaders: Caesar</t>
+  </si>
+  <si>
+    <t>9 Mar, 2018</t>
+  </si>
+  <si>
+    <t>CDN$ 51.99</t>
+  </si>
+  <si>
+    <t>Business tour. Great Leaders: Lincoln</t>
+  </si>
+  <si>
+    <t>16 Apr, 2018</t>
+  </si>
+  <si>
+    <t>CONFLICT OF NATIONS: WORLD WAR 3 Army Pack</t>
+  </si>
+  <si>
+    <t>15 Mar, 2018</t>
+  </si>
+  <si>
+    <t>Children of Morta: Complete Edition</t>
+  </si>
+  <si>
+    <t>CDN$ 124.99</t>
+  </si>
+  <si>
+    <t>Cities: Skylines Collection</t>
+  </si>
+  <si>
+    <t>CDN$ 137.99</t>
+  </si>
+  <si>
+    <t>Conqueror's Blade - Imperial Heir Collector’s Pack</t>
+  </si>
+  <si>
+    <t>28 Jan, 2021</t>
+  </si>
+  <si>
+    <t>CDN$ 26.99</t>
+  </si>
+  <si>
+    <t>Crossout - Insomnia Pack</t>
+  </si>
+  <si>
+    <t>21 Aug, 2018</t>
+  </si>
+  <si>
+    <t>CDN$ 99.99</t>
+  </si>
+  <si>
+    <t>Crossout - Phantom</t>
+  </si>
+  <si>
+    <t>22 Oct, 2020</t>
+  </si>
+  <si>
+    <t>CDN$ 31.99</t>
+  </si>
+  <si>
+    <t>DCS: F-86F Sabre</t>
+  </si>
+  <si>
+    <t>8 Aug, 2014</t>
+  </si>
+  <si>
+    <t>Destiny 2: Beyond Light</t>
+  </si>
+  <si>
+    <t>10 Nov, 2020</t>
   </si>
   <si>
     <t>CDN$ 329.07</t>
   </si>
   <si>
-    <t>Brawlhalla - Battle Pass Season 6</t>
-  </si>
-  <si>
-    <t>22 Jun, 2022</t>
-  </si>
-  <si>
-    <t>CDN$ 49.99</t>
-  </si>
-  <si>
-    <t>Brawlhalla - Collectors Pack</t>
-  </si>
-  <si>
-    <t>30 Apr, 2014</t>
-  </si>
-  <si>
-    <t>CDN$ 109.99</t>
-  </si>
-  <si>
-    <t>Century - Arisen Pack</t>
-  </si>
-  <si>
-    <t>17 Dec, 2021</t>
-  </si>
-  <si>
-    <t>CDN$ 31.99</t>
-  </si>
-  <si>
-    <t>Century - Colossus Deluxe Pack</t>
-  </si>
-  <si>
-    <t>7 Apr, 2022</t>
-  </si>
-  <si>
-    <t>CDN$ 46.22</t>
-  </si>
-  <si>
-    <t>Cities: Skylines Collection</t>
-  </si>
-  <si>
-    <t>CDN$ 28.99
-CDN$ 23.19</t>
-  </si>
-  <si>
-    <t>Conqueror's Blade - Battle Saga Collector's Pack</t>
-  </si>
-  <si>
-    <t>6 May, 2021</t>
+    <t>Destiny 2: Bungie 30th Anniversary Pack</t>
+  </si>
+  <si>
+    <t>7 Dec, 2021</t>
+  </si>
+  <si>
+    <t>CDN$ 79.48</t>
+  </si>
+  <si>
+    <t>Destiny 2: Legacy Collection</t>
+  </si>
+  <si>
+    <t>18 Jan, 2022</t>
+  </si>
+  <si>
+    <t>CDN$ 44.97</t>
+  </si>
+  <si>
+    <t>Destiny 2: Season of the Haunted Silver Bundle</t>
+  </si>
+  <si>
+    <t>24 May, 2022</t>
+  </si>
+  <si>
+    <t>CDN$ 74.99</t>
+  </si>
+  <si>
+    <t>Destiny 2: The Witch Queen</t>
+  </si>
+  <si>
+    <t>22 Feb, 2022</t>
+  </si>
+  <si>
+    <t>CDN$ 39.99</t>
+  </si>
+  <si>
+    <t>Destiny 2: The Witch Queen Deluxe + Bungie 30th Anniversary Bundle</t>
+  </si>
+  <si>
+    <t>CDN$ 20.49
+CDN$ 18.44</t>
+  </si>
+  <si>
+    <t>Destiny 2: The Witch Queen Deluxe Edition</t>
+  </si>
+  <si>
+    <t>CDN$ 17.49</t>
+  </si>
+  <si>
+    <t>Destiny 2: The Witch Queen Deluxe Edition Upgrade</t>
+  </si>
+  <si>
+    <t>CDN$ 63.99</t>
+  </si>
+  <si>
+    <t>Fire and Maneuver | Expansion: American Civil War</t>
+  </si>
+  <si>
+    <t>15 Jul, 2022</t>
+  </si>
+  <si>
+    <t>CDN$ 37.49</t>
+  </si>
+  <si>
+    <t>Fire and Maneuver | Music Pack: Franco-Prussian War</t>
+  </si>
+  <si>
+    <t>CDN$ 45.49</t>
+  </si>
+  <si>
+    <t>Fire and Maneuver | Starter Pack: European Empires</t>
+  </si>
+  <si>
+    <t>CDN$ 44.73</t>
+  </si>
+  <si>
+    <t>Fishing Planet: Congo Discovery Pack</t>
+  </si>
+  <si>
+    <t>30 Nov, 2021</t>
+  </si>
+  <si>
+    <t>CDN$ 33.99</t>
+  </si>
+  <si>
+    <t>Fishing Planet: Golden Dragon Pack</t>
+  </si>
+  <si>
+    <t>15 Jun, 2018</t>
+  </si>
+  <si>
+    <t>CDN$ 11.49</t>
+  </si>
+  <si>
+    <t>Fishing Planet: Wild Africa Pack</t>
+  </si>
+  <si>
+    <t>11 Jan, 2022</t>
+  </si>
+  <si>
+    <t>Grand Theft Auto V: Premium Edition</t>
+  </si>
+  <si>
+    <t>CDN$ 54.47
+CDN$ 24.45</t>
+  </si>
+  <si>
+    <t>Grand Theft Auto V: Premium Edition &amp; Great White Shark Card Bundle</t>
   </si>
   <si>
     <t>CDN$ 18.99</t>
   </si>
   <si>
-    <t>Dark Deception Complete</t>
-  </si>
-  <si>
-    <t>29 Jan, 2019</t>
-  </si>
-  <si>
-    <t>Destiny 2: Beyond Light</t>
-  </si>
-  <si>
-    <t>10 Nov, 2020</t>
-  </si>
-  <si>
-    <t>CDN$ 33.99</t>
-  </si>
-  <si>
-    <t>Destiny 2: Bungie 30th Anniversary Pack</t>
-  </si>
-  <si>
-    <t>7 Dec, 2021</t>
-  </si>
-  <si>
-    <t>CDN$ 21.99</t>
-  </si>
-  <si>
-    <t>Destiny 2: Season of the Haunted Silver Bundle</t>
-  </si>
-  <si>
-    <t>24 May, 2022</t>
-  </si>
-  <si>
-    <t>CDN$ 25.99</t>
-  </si>
-  <si>
-    <t>Destiny 2: The Witch Queen</t>
-  </si>
-  <si>
-    <t>22 Feb, 2022</t>
-  </si>
-  <si>
-    <t>CDN$ 11.49</t>
-  </si>
-  <si>
-    <t>Destiny 2: The Witch Queen Deluxe + Bungie 30th Anniversary Bundle</t>
-  </si>
-  <si>
-    <t>CDN$ 124.99</t>
-  </si>
-  <si>
-    <t>Destiny 2: The Witch Queen Deluxe Edition</t>
-  </si>
-  <si>
-    <t>CDN$ 8.99</t>
-  </si>
-  <si>
-    <t>Destiny 2: The Witch Queen Deluxe Edition Upgrade</t>
-  </si>
-  <si>
-    <t>CDN$ 22.79</t>
-  </si>
-  <si>
-    <t>Destiny 2: Throne of Atheon Emote Bundle</t>
-  </si>
-  <si>
-    <t>21 May, 2021</t>
-  </si>
-  <si>
-    <t>Destiny 2: Triumphant Silver Bundle</t>
-  </si>
-  <si>
-    <t>CDN$ 137.99</t>
-  </si>
-  <si>
-    <t>Emily Wants To Play</t>
-  </si>
-  <si>
-    <t>10 Dec, 2015</t>
-  </si>
-  <si>
-    <t>CDN$ 74.29</t>
-  </si>
-  <si>
-    <t>Emily Wants to Play Too</t>
-  </si>
-  <si>
-    <t>13 Dec, 2017</t>
-  </si>
-  <si>
-    <t>CDN$ 13.49</t>
-  </si>
-  <si>
-    <t>Fishing Planet - Sport Bottom Pack</t>
-  </si>
-  <si>
-    <t>27 Nov, 2019</t>
-  </si>
-  <si>
-    <t>CDN$ 79.48</t>
-  </si>
-  <si>
-    <t>Grand Theft Auto V: Premium Edition</t>
-  </si>
-  <si>
-    <t>CDN$ 14.99</t>
-  </si>
-  <si>
     <t>Grand Theft Auto V: Premium Edition &amp; Whale Shark Card Bundle</t>
   </si>
   <si>
-    <t>CDN$ 17.49</t>
+    <t>CDN$ 27.99</t>
+  </si>
+  <si>
+    <t>Hidden Through Time - Deluxe Edition</t>
+  </si>
+  <si>
+    <t>CDN$ 12.49</t>
   </si>
   <si>
     <t>House Builder</t>
@@ -221,62 +262,77 @@
     <t>11 Nov, 2021</t>
   </si>
   <si>
+    <t>CDN$ 39.96
+CDN$ 15.96</t>
+  </si>
+  <si>
+    <t>Idle Champions - Bruenor Starter Pack</t>
+  </si>
+  <si>
+    <t>20 Sep, 2017</t>
+  </si>
+  <si>
     <t>CDN$ 6.99</t>
   </si>
   <si>
-    <t>Idle Champions - Bruenor Starter Pack</t>
-  </si>
-  <si>
-    <t>20 Sep, 2017</t>
+    <t>Idle Champions - Nayeli Starter Pack</t>
+  </si>
+  <si>
+    <t>CDN$ 33.27</t>
+  </si>
+  <si>
+    <t>Idle Champions - Polymorphed Orkira Skin &amp; Feat Pack</t>
+  </si>
+  <si>
+    <t>4 May, 2022</t>
+  </si>
+  <si>
+    <t>CDN$ 28.99</t>
+  </si>
+  <si>
+    <t>Idle Champions - Steampunk Nordom the Modron Theme Pack</t>
+  </si>
+  <si>
+    <t>18 May, 2022</t>
+  </si>
+  <si>
+    <t>CDN$ 11.49
+CDN$ 8.04</t>
+  </si>
+  <si>
+    <t>Life is Strange 2 Complete Season</t>
+  </si>
+  <si>
+    <t>CDN$ 59.37</t>
+  </si>
+  <si>
+    <t>Lost Ark Vanquisher Starter Pack</t>
+  </si>
+  <si>
+    <t>11 Feb, 2022</t>
+  </si>
+  <si>
+    <t>CDN$ 83.99</t>
+  </si>
+  <si>
+    <t>Minimalist Mash-Up Bundle</t>
+  </si>
+  <si>
+    <t>CDN$ 87.03
+CDN$ 22.59</t>
+  </si>
+  <si>
+    <t>OUTRIDERS WORLDSLAYER</t>
   </si>
   <si>
     <t>CDN$ 17.49
 CDN$ 13.99</t>
   </si>
   <si>
-    <t>Idle Champions - Gladiator Havilar Theme Pack</t>
-  </si>
-  <si>
-    <t>13 Jul, 2022</t>
-  </si>
-  <si>
-    <t>CDN$ 5.69</t>
-  </si>
-  <si>
-    <t>Lost Ark Apprentice Starter Pack</t>
-  </si>
-  <si>
-    <t>11 Feb, 2022</t>
-  </si>
-  <si>
-    <t>CDN$ 99.99</t>
-  </si>
-  <si>
-    <t>Lost Ark Vanquisher Starter Pack</t>
-  </si>
-  <si>
-    <t>Neverwinter Nights: Complete Adventures</t>
-  </si>
-  <si>
-    <t>CDN$ 83.99</t>
-  </si>
-  <si>
-    <t>OUTRIDERS WORLDSLAYER</t>
-  </si>
-  <si>
-    <t>CDN$ 10.99</t>
-  </si>
-  <si>
-    <t>Old School RuneScape 1-Month Membership</t>
-  </si>
-  <si>
-    <t>24 Feb, 2021</t>
-  </si>
-  <si>
-    <t>Order of Battle: Allies Defiant</t>
-  </si>
-  <si>
-    <t>28 Jan, 2021</t>
+    <t>Pajama Sam Complete Pack</t>
+  </si>
+  <si>
+    <t>CDN$ 3.39</t>
   </si>
   <si>
     <t>Poppy Playtime - Chapter 2</t>
@@ -285,19 +341,8 @@
     <t>5 May, 2022</t>
   </si>
   <si>
-    <t>CDN$ 37.49</t>
-  </si>
-  <si>
-    <t>RuneScape: 15 Treasure Hunter Keys</t>
-  </si>
-  <si>
-    <t>SMITE - Best Sellers Bundle</t>
-  </si>
-  <si>
-    <t>16 Nov, 2018</t>
-  </si>
-  <si>
-    <t>CDN$ 59.37</t>
+    <t>CDN$ 15.86
+CDN$ 11.03</t>
   </si>
   <si>
     <t>SMITE® - Ultimate God Pack</t>
@@ -306,47 +351,11 @@
     <t>8 Sep, 2015</t>
   </si>
   <si>
-    <t>CDN$ 78.72</t>
-  </si>
-  <si>
-    <t>Sport Casting Bass Pack</t>
-  </si>
-  <si>
-    <t>27 May, 2016</t>
-  </si>
-  <si>
-    <t>CDN$ 26.99</t>
-  </si>
-  <si>
-    <t>Sport Float Pack</t>
-  </si>
-  <si>
-    <t>Sport Outfit Pack</t>
-  </si>
-  <si>
-    <t>CDN$ 5.49</t>
-  </si>
-  <si>
-    <t>Sport Spinning Trout Pack</t>
-  </si>
-  <si>
-    <t>Sport Topwater Night Pack</t>
-  </si>
-  <si>
-    <t>17 Nov, 2017</t>
-  </si>
-  <si>
-    <t>CDN$ 56.99</t>
-  </si>
-  <si>
-    <t>Sport Ultralight Panfish Pack</t>
-  </si>
-  <si>
-    <t>THE COMPLETE SUPERHOT BUNDLE</t>
-  </si>
-  <si>
-    <t>CDN$ 11.49
-CDN$ 4.59</t>
+    <t>CDN$ 33.99
+CDN$ 8.49</t>
+  </si>
+  <si>
+    <t>Sudden Strike 4 - Complete Collection</t>
   </si>
   <si>
     <t>The Cycle: Frontier - Elite Pack</t>
@@ -355,34 +364,47 @@
     <t>8 Jun, 2022</t>
   </si>
   <si>
-    <t>CDN$ 32.99</t>
-  </si>
-  <si>
-    <t>The Cycle: Frontier - Professional Pack</t>
-  </si>
-  <si>
-    <t>The Orange Box</t>
-  </si>
-  <si>
-    <t>10 Oct, 2007</t>
-  </si>
-  <si>
-    <t>Warframe: Garuda Prime Access - Accessories Pack</t>
-  </si>
-  <si>
-    <t>28 Mar, 2022</t>
-  </si>
-  <si>
-    <t>Warframe: Tennocon 2022 Digital Pack</t>
-  </si>
-  <si>
-    <t>9 Jun, 2022</t>
+    <t>CDN$ 7.99</t>
+  </si>
+  <si>
+    <t>Upgrade from Fantasy Grounds to Fantasy Grounds Unity (Standard license)</t>
+  </si>
+  <si>
+    <t>War Thunder - F-5C Pack</t>
+  </si>
+  <si>
+    <t>7 Jun, 2021</t>
+  </si>
+  <si>
+    <t>CDN$ 72.99</t>
+  </si>
+  <si>
+    <t>War Thunder - German Beginner's Pack</t>
+  </si>
+  <si>
+    <t>15 Jun, 2022</t>
+  </si>
+  <si>
+    <t>CDN$ 10.29</t>
+  </si>
+  <si>
+    <t>Warframe: Khora Prime Access - Accessories Pack</t>
+  </si>
+  <si>
+    <t>16 Jul, 2022</t>
+  </si>
+  <si>
+    <t>CDN$ 28.99
+CDN$ 20.29</t>
+  </si>
+  <si>
+    <t>Warframe: Khora Prime Access - Whipclaw Pack</t>
+  </si>
+  <si>
+    <t>CDN$ 6.39</t>
   </si>
   <si>
     <t>Zaccaria Pinball - POSTAL Redux Pinball Pack</t>
-  </si>
-  <si>
-    <t>Game Price</t>
   </si>
 </sst>
 </file>
@@ -754,7 +776,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -772,66 +796,66 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>119</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -842,147 +866,144 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
         <v>35</v>
       </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
         <v>38</v>
       </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
         <v>41</v>
       </c>
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
         <v>43</v>
-      </c>
-      <c r="B16" t="s">
-        <v>39</v>
       </c>
       <c r="C16" t="s">
         <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -990,55 +1011,55 @@
         <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
         <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1052,7 +1073,7 @@
         <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1060,35 +1081,41 @@
         <v>57</v>
       </c>
       <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s">
         <v>58</v>
       </c>
-      <c r="C22" t="s">
-        <v>59</v>
-      </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
         <v>60</v>
       </c>
-      <c r="C23" t="s">
-        <v>61</v>
-      </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
         <v>62</v>
       </c>
       <c r="C24" t="s">
         <v>63</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1102,7 +1129,7 @@
         <v>66</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1113,88 +1140,82 @@
         <v>68</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" t="s">
         <v>70</v>
       </c>
-      <c r="B27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" t="s">
-        <v>72</v>
-      </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>73</v>
-      </c>
-      <c r="B28" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>76</v>
-      </c>
-      <c r="B29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" t="s">
         <v>74</v>
       </c>
-      <c r="C29" t="s">
-        <v>66</v>
-      </c>
       <c r="D29" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" t="s">
         <v>79</v>
       </c>
-      <c r="C31" t="s">
-        <v>80</v>
-      </c>
       <c r="D31" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" t="s">
         <v>81</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>82</v>
       </c>
-      <c r="C32" t="s">
-        <v>72</v>
-      </c>
       <c r="D32" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1202,13 +1223,13 @@
         <v>83</v>
       </c>
       <c r="B33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" t="s">
         <v>84</v>
       </c>
-      <c r="C33" t="s">
-        <v>12</v>
-      </c>
       <c r="D33" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1222,7 +1243,7 @@
         <v>87</v>
       </c>
       <c r="D34" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1230,215 +1251,235 @@
         <v>88</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="C35" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="D35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>89</v>
-      </c>
-      <c r="B36" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D36" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C37" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>95</v>
-      </c>
-      <c r="B38" t="s">
         <v>96</v>
       </c>
       <c r="C38" t="s">
         <v>97</v>
       </c>
       <c r="D38" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>98</v>
       </c>
-      <c r="B39" t="s">
-        <v>96</v>
-      </c>
       <c r="C39" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="D39" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>99</v>
-      </c>
-      <c r="B40" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D40" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="D41" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D42" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>105</v>
-      </c>
-      <c r="B43" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="D43" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>109</v>
+      </c>
+      <c r="B44" t="s">
+        <v>110</v>
       </c>
       <c r="C44" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D44" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>108</v>
-      </c>
-      <c r="B45" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C45" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D45" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B46" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C46" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="D46" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B47" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C47" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="D47" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B48" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C48" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="D48" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C49" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="D49" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCACA9EA-661F-4EBB-84B4-DFD12C5B9237}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="52.77734375" customWidth="1"/>
+    <col min="2" max="2" width="32.77734375" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+    <col min="4" max="4" width="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>